<commit_message>
update metrics and backgroud
</commit_message>
<xml_diff>
--- a/Análise/Vendas/Vendas - Ecommerce.xlsx
+++ b/Análise/Vendas/Vendas - Ecommerce.xlsx
@@ -5,13 +5,15 @@
   <sheets>
     <sheet state="visible" name="Vendas" sheetId="1" r:id="rId4"/>
   </sheets>
-  <definedNames/>
+  <definedNames>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Vendas!$A$1:$J$395</definedName>
+  </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1087" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1192" uniqueCount="44">
   <si>
     <t>ID da Venda</t>
   </si>
@@ -179,7 +181,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -189,6 +191,7 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -7735,7 +7738,7 @@
       <c r="F253" s="1">
         <v>45.99</v>
       </c>
-      <c r="H253" s="1">
+      <c r="H253" s="3">
         <v>137.97</v>
       </c>
       <c r="I253" s="1" t="s">
@@ -7764,7 +7767,7 @@
       <c r="F254" s="1">
         <v>55.4</v>
       </c>
-      <c r="H254" s="1">
+      <c r="H254" s="3">
         <v>221.6</v>
       </c>
       <c r="I254" s="1" t="s">
@@ -7793,7 +7796,7 @@
       <c r="F255" s="1">
         <v>150.75</v>
       </c>
-      <c r="H255" s="1">
+      <c r="H255" s="3">
         <v>301.5</v>
       </c>
       <c r="I255" s="1" t="s">
@@ -7822,7 +7825,7 @@
       <c r="F256" s="1">
         <v>70.5</v>
       </c>
-      <c r="H256" s="1">
+      <c r="H256" s="3">
         <v>352.5</v>
       </c>
       <c r="I256" s="1" t="s">
@@ -7851,8 +7854,8 @@
       <c r="F257" s="1">
         <v>45.2</v>
       </c>
-      <c r="H257" s="1">
-        <v>271.2</v>
+      <c r="H257" s="3">
+        <v>271.20000000000005</v>
       </c>
       <c r="I257" s="1" t="s">
         <v>14</v>
@@ -7880,7 +7883,7 @@
       <c r="F258" s="1">
         <v>250.99</v>
       </c>
-      <c r="H258" s="1">
+      <c r="H258" s="3">
         <v>752.97</v>
       </c>
       <c r="I258" s="1" t="s">
@@ -7909,7 +7912,7 @@
       <c r="F259" s="1">
         <v>120.75</v>
       </c>
-      <c r="H259" s="1">
+      <c r="H259" s="3">
         <v>483.0</v>
       </c>
       <c r="I259" s="1" t="s">
@@ -8620,7 +8623,7 @@
         <v>283.0</v>
       </c>
       <c r="B284" s="2">
-        <v>45433.82148148148</v>
+        <v>45372.82148148148</v>
       </c>
       <c r="C284" s="1">
         <v>15.0</v>
@@ -8649,7 +8652,7 @@
         <v>284.0</v>
       </c>
       <c r="B285" s="2">
-        <v>45437.708125</v>
+        <v>45376.708125</v>
       </c>
       <c r="C285" s="1">
         <v>11.0</v>
@@ -8692,7 +8695,7 @@
       <c r="F286" s="1">
         <v>30.12</v>
       </c>
-      <c r="H286" s="1">
+      <c r="H286" s="3">
         <v>150.6</v>
       </c>
       <c r="I286" s="1" t="s">
@@ -8765,7 +8768,7 @@
         <v>288.0</v>
       </c>
       <c r="B289" s="2">
-        <v>45475.26664351852</v>
+        <v>45353.26664351852</v>
       </c>
       <c r="C289" s="1">
         <v>15.0</v>
@@ -8794,7 +8797,7 @@
         <v>289.0</v>
       </c>
       <c r="B290" s="2">
-        <v>45464.01792824074</v>
+        <v>45372.01792824074</v>
       </c>
       <c r="C290" s="1">
         <v>3.0</v>
@@ -8852,7 +8855,7 @@
         <v>291.0</v>
       </c>
       <c r="B292" s="2">
-        <v>45434.98903935185</v>
+        <v>45404.98903935185</v>
       </c>
       <c r="C292" s="1">
         <v>20.0</v>
@@ -8953,7 +8956,7 @@
       <c r="F295" s="1">
         <v>903.25</v>
       </c>
-      <c r="H295" s="1">
+      <c r="H295" s="3">
         <v>5419.5</v>
       </c>
       <c r="I295" s="1" t="s">
@@ -9011,8 +9014,8 @@
       <c r="F297" s="1">
         <v>433.35</v>
       </c>
-      <c r="H297" s="1">
-        <v>2600.1</v>
+      <c r="H297" s="3">
+        <v>2600.1000000000004</v>
       </c>
       <c r="I297" s="1" t="s">
         <v>11</v>
@@ -9055,7 +9058,7 @@
         <v>298.0</v>
       </c>
       <c r="B299" s="2">
-        <v>45492.716886574075</v>
+        <v>45401.716886574075</v>
       </c>
       <c r="C299" s="1">
         <v>10.0</v>
@@ -9084,7 +9087,7 @@
         <v>299.0</v>
       </c>
       <c r="B300" s="2">
-        <v>45446.0</v>
+        <v>45385.0</v>
       </c>
       <c r="C300" s="1">
         <v>11.0</v>
@@ -9127,7 +9130,7 @@
       <c r="F301" s="1">
         <v>57.43</v>
       </c>
-      <c r="H301" s="1">
+      <c r="H301" s="3">
         <v>287.15</v>
       </c>
       <c r="I301" s="1" t="s">
@@ -9171,7 +9174,7 @@
         <v>302.0</v>
       </c>
       <c r="B303" s="2">
-        <v>45467.74513888889</v>
+        <v>45406.74513888889</v>
       </c>
       <c r="C303" s="1">
         <v>7.0</v>
@@ -9258,7 +9261,7 @@
         <v>305.0</v>
       </c>
       <c r="B306" s="2">
-        <v>45486.86865740741</v>
+        <v>45425.86865740741</v>
       </c>
       <c r="C306" s="1">
         <v>20.0</v>
@@ -9287,7 +9290,7 @@
         <v>306.0</v>
       </c>
       <c r="B307" s="2">
-        <v>45448.040671296294</v>
+        <v>45417.040671296294</v>
       </c>
       <c r="C307" s="1">
         <v>4.0</v>
@@ -9316,7 +9319,7 @@
         <v>307.0</v>
       </c>
       <c r="B308" s="2">
-        <v>45479.01912037037</v>
+        <v>45418.01912037037</v>
       </c>
       <c r="C308" s="1">
         <v>20.0</v>
@@ -9345,7 +9348,7 @@
         <v>308.0</v>
       </c>
       <c r="B309" s="2">
-        <v>45480.823796296296</v>
+        <v>45419.823796296296</v>
       </c>
       <c r="C309" s="1">
         <v>20.0</v>
@@ -9417,7 +9420,7 @@
       <c r="F311" s="1">
         <v>115.69</v>
       </c>
-      <c r="H311" s="1">
+      <c r="H311" s="3">
         <v>1041.21</v>
       </c>
       <c r="I311" s="1" t="s">
@@ -9432,7 +9435,7 @@
         <v>311.0</v>
       </c>
       <c r="B312" s="2">
-        <v>45497.97075231482</v>
+        <v>45346.97075231482</v>
       </c>
       <c r="C312" s="1">
         <v>16.0</v>
@@ -9461,7 +9464,7 @@
         <v>312.0</v>
       </c>
       <c r="B313" s="2">
-        <v>45518.996875</v>
+        <v>45336.996875</v>
       </c>
       <c r="C313" s="1">
         <v>21.0</v>
@@ -9490,7 +9493,7 @@
         <v>313.0</v>
       </c>
       <c r="B314" s="2">
-        <v>45510.390706018516</v>
+        <v>45328.390706018516</v>
       </c>
       <c r="C314" s="1">
         <v>14.0</v>
@@ -9533,8 +9536,8 @@
       <c r="F315" s="1">
         <v>30.12</v>
       </c>
-      <c r="H315" s="1">
-        <v>150.6</v>
+      <c r="H315" s="3">
+        <v>90.36</v>
       </c>
       <c r="I315" s="1" t="s">
         <v>11</v>
@@ -9562,7 +9565,7 @@
       <c r="F316" s="1">
         <v>699.99</v>
       </c>
-      <c r="H316" s="1">
+      <c r="H316" s="3">
         <v>3499.95</v>
       </c>
       <c r="I316" s="1" t="s">
@@ -9586,13 +9589,13 @@
         <v>40</v>
       </c>
       <c r="E317" s="1">
-        <v>3.0</v>
+        <v>10.0</v>
       </c>
       <c r="F317" s="1">
         <v>1200.5</v>
       </c>
-      <c r="H317" s="1">
-        <v>3601.5</v>
+      <c r="H317" s="3">
+        <v>12005.0</v>
       </c>
       <c r="I317" s="1" t="s">
         <v>11</v>
@@ -9620,7 +9623,7 @@
       <c r="F318" s="1">
         <v>679.99</v>
       </c>
-      <c r="H318" s="1">
+      <c r="H318" s="3">
         <v>2719.96</v>
       </c>
       <c r="I318" s="1" t="s">
@@ -9649,7 +9652,7 @@
       <c r="F319" s="1">
         <v>1199.99</v>
       </c>
-      <c r="H319" s="1">
+      <c r="H319" s="3">
         <v>2399.98</v>
       </c>
       <c r="I319" s="1" t="s">
@@ -9667,7 +9670,7 @@
         <v>45306.57444444444</v>
       </c>
       <c r="C320" s="1">
-        <v>9.0</v>
+        <v>20.0</v>
       </c>
       <c r="D320" s="1" t="s">
         <v>24</v>
@@ -9678,7 +9681,7 @@
       <c r="F320" s="1">
         <v>1350.75</v>
       </c>
-      <c r="H320" s="1">
+      <c r="H320" s="3">
         <v>1350.75</v>
       </c>
       <c r="I320" s="1" t="s">
@@ -9707,7 +9710,7 @@
       <c r="F321" s="1">
         <v>649.99</v>
       </c>
-      <c r="H321" s="1">
+      <c r="H321" s="3">
         <v>1949.97</v>
       </c>
       <c r="I321" s="1" t="s">
@@ -9736,7 +9739,7 @@
       <c r="F322" s="1">
         <v>1149.99</v>
       </c>
-      <c r="H322" s="1">
+      <c r="H322" s="3">
         <v>4599.96</v>
       </c>
       <c r="I322" s="1" t="s">
@@ -9765,7 +9768,7 @@
       <c r="F323" s="1">
         <v>950.5</v>
       </c>
-      <c r="H323" s="1">
+      <c r="H323" s="3">
         <v>1901.0</v>
       </c>
       <c r="I323" s="1" t="s">
@@ -9794,8 +9797,8 @@
       <c r="F324" s="1">
         <v>699.99</v>
       </c>
-      <c r="H324" s="1">
-        <v>4199.94</v>
+      <c r="H324" s="3">
+        <v>4199.9400000000005</v>
       </c>
       <c r="I324" s="1" t="s">
         <v>22</v>
@@ -9823,7 +9826,7 @@
       <c r="F325" s="1">
         <v>1100.75</v>
       </c>
-      <c r="H325" s="1">
+      <c r="H325" s="3">
         <v>5503.75</v>
       </c>
       <c r="I325" s="1" t="s">
@@ -10766,7 +10769,7 @@
         <v>357.0</v>
       </c>
       <c r="B358" s="2">
-        <v>45435.43578703704</v>
+        <v>45314.43578703704</v>
       </c>
       <c r="C358" s="1">
         <v>22.0</v>
@@ -10780,7 +10783,7 @@
       <c r="F358" s="1">
         <v>750.75</v>
       </c>
-      <c r="H358" s="1">
+      <c r="H358" s="3">
         <v>3003.0</v>
       </c>
       <c r="I358" s="1" t="s">
@@ -10795,7 +10798,7 @@
         <v>358.0</v>
       </c>
       <c r="B359" s="2">
-        <v>45439.621770833335</v>
+        <v>45318.621770833335</v>
       </c>
       <c r="C359" s="1">
         <v>5.0</v>
@@ -10804,13 +10807,13 @@
         <v>18</v>
       </c>
       <c r="E359" s="1">
-        <v>2.0</v>
+        <v>20.0</v>
       </c>
       <c r="F359" s="1">
         <v>899.99</v>
       </c>
-      <c r="H359" s="1">
-        <v>1799.98</v>
+      <c r="H359" s="3">
+        <v>17999.8</v>
       </c>
       <c r="I359" s="1" t="s">
         <v>11</v>
@@ -10824,7 +10827,7 @@
         <v>359.0</v>
       </c>
       <c r="B360" s="2">
-        <v>45443.471134259256</v>
+        <v>45382.471134259256</v>
       </c>
       <c r="C360" s="1">
         <v>23.0</v>
@@ -10848,7 +10851,1023 @@
         <v>23</v>
       </c>
     </row>
+    <row r="361">
+      <c r="A361" s="1">
+        <v>360.0</v>
+      </c>
+      <c r="B361" s="2">
+        <v>45319.53873842592</v>
+      </c>
+      <c r="C361" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="D361" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E361" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="F361" s="1">
+        <v>699.99</v>
+      </c>
+      <c r="H361" s="1">
+        <v>3499.95</v>
+      </c>
+      <c r="I361" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J361" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" s="1">
+        <v>361.0</v>
+      </c>
+      <c r="B362" s="2">
+        <v>45292.779965277776</v>
+      </c>
+      <c r="C362" s="1">
+        <v>25.0</v>
+      </c>
+      <c r="D362" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E362" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="F362" s="1">
+        <v>1100.75</v>
+      </c>
+      <c r="H362" s="1">
+        <v>3302.25</v>
+      </c>
+      <c r="I362" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J362" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" s="1">
+        <v>362.0</v>
+      </c>
+      <c r="B363" s="2">
+        <v>45295.621770833335</v>
+      </c>
+      <c r="C363" s="1">
+        <v>22.0</v>
+      </c>
+      <c r="D363" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E363" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="F363" s="1">
+        <v>750.75</v>
+      </c>
+      <c r="H363" s="1">
+        <v>750.75</v>
+      </c>
+      <c r="I363" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J363" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" s="1">
+        <v>363.0</v>
+      </c>
+      <c r="B364" s="2">
+        <v>45298.43578703704</v>
+      </c>
+      <c r="C364" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="D364" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E364" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="F364" s="1">
+        <v>899.99</v>
+      </c>
+      <c r="H364" s="1">
+        <v>1799.98</v>
+      </c>
+      <c r="I364" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J364" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" s="1">
+        <v>364.0</v>
+      </c>
+      <c r="B365" s="2">
+        <v>45301.56884259259</v>
+      </c>
+      <c r="C365" s="1">
+        <v>23.0</v>
+      </c>
+      <c r="D365" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E365" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="F365" s="1">
+        <v>450.5</v>
+      </c>
+      <c r="H365" s="1">
+        <v>1802.0</v>
+      </c>
+      <c r="I365" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J365" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" s="1">
+        <v>365.0</v>
+      </c>
+      <c r="B366" s="2">
+        <v>45304.82842592592</v>
+      </c>
+      <c r="C366" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="D366" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E366" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="F366" s="1">
+        <v>699.99</v>
+      </c>
+      <c r="H366" s="1">
+        <v>4199.94</v>
+      </c>
+      <c r="I366" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J366" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" s="1">
+        <v>366.0</v>
+      </c>
+      <c r="B367" s="2">
+        <v>45307.67340277778</v>
+      </c>
+      <c r="C367" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="D367" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E367" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="F367" s="1">
+        <v>599.99</v>
+      </c>
+      <c r="H367" s="1">
+        <v>1799.97</v>
+      </c>
+      <c r="I367" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J367" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" s="1">
+        <v>367.0</v>
+      </c>
+      <c r="B368" s="2">
+        <v>45310.38579861111</v>
+      </c>
+      <c r="C368" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="D368" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E368" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="F368" s="1">
+        <v>1350.75</v>
+      </c>
+      <c r="H368" s="1">
+        <v>1350.75</v>
+      </c>
+      <c r="I368" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J368" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" s="1">
+        <v>368.0</v>
+      </c>
+      <c r="B369" s="2">
+        <v>45314.60266203704</v>
+      </c>
+      <c r="C369" s="1">
+        <v>25.0</v>
+      </c>
+      <c r="D369" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E369" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="F369" s="1">
+        <v>1149.99</v>
+      </c>
+      <c r="H369" s="1">
+        <v>4599.96</v>
+      </c>
+      <c r="I369" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J369" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" s="1">
+        <v>369.0</v>
+      </c>
+      <c r="B370" s="2">
+        <v>45318.4828587963</v>
+      </c>
+      <c r="C370" s="1">
+        <v>28.0</v>
+      </c>
+      <c r="D370" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E370" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="F370" s="1">
+        <v>950.5</v>
+      </c>
+      <c r="H370" s="1">
+        <v>1901.0</v>
+      </c>
+      <c r="I370" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J370" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" s="1">
+        <v>370.0</v>
+      </c>
+      <c r="B371" s="2">
+        <v>45292.779594907406</v>
+      </c>
+      <c r="C371" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="D371" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E371" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="F371" s="1">
+        <v>849.99</v>
+      </c>
+      <c r="H371" s="1">
+        <v>4249.95</v>
+      </c>
+      <c r="I371" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J371" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" s="1">
+        <v>371.0</v>
+      </c>
+      <c r="B372" s="2">
+        <v>45296.67644675926</v>
+      </c>
+      <c r="C372" s="1">
+        <v>23.0</v>
+      </c>
+      <c r="D372" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E372" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="F372" s="1">
+        <v>450.5</v>
+      </c>
+      <c r="H372" s="1">
+        <v>1351.5</v>
+      </c>
+      <c r="I372" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J372" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" s="1">
+        <v>372.0</v>
+      </c>
+      <c r="B373" s="2">
+        <v>45300.394594907404</v>
+      </c>
+      <c r="C373" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="D373" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E373" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="F373" s="1">
+        <v>679.99</v>
+      </c>
+      <c r="H373" s="1">
+        <v>2719.96</v>
+      </c>
+      <c r="I373" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J373" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" s="1">
+        <v>373.0</v>
+      </c>
+      <c r="B374" s="2">
+        <v>45303.561898148146</v>
+      </c>
+      <c r="C374" s="1">
+        <v>25.0</v>
+      </c>
+      <c r="D374" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E374" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="F374" s="1">
+        <v>1199.99</v>
+      </c>
+      <c r="H374" s="1">
+        <v>2399.98</v>
+      </c>
+      <c r="I374" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J374" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" s="1">
+        <v>374.0</v>
+      </c>
+      <c r="B375" s="2">
+        <v>45306.82148148148</v>
+      </c>
+      <c r="C375" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="D375" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E375" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="F375" s="1">
+        <v>1350.75</v>
+      </c>
+      <c r="H375" s="1">
+        <v>1350.75</v>
+      </c>
+      <c r="I375" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J375" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" s="1">
+        <v>375.0</v>
+      </c>
+      <c r="B376" s="2">
+        <v>45310.71506944444</v>
+      </c>
+      <c r="C376" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="D376" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E376" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="F376" s="1">
+        <v>599.99</v>
+      </c>
+      <c r="H376" s="1">
+        <v>1799.97</v>
+      </c>
+      <c r="I376" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J376" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" s="1">
+        <v>376.0</v>
+      </c>
+      <c r="B377" s="2">
+        <v>45315.43578703704</v>
+      </c>
+      <c r="C377" s="1">
+        <v>22.0</v>
+      </c>
+      <c r="D377" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E377" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="F377" s="1">
+        <v>750.75</v>
+      </c>
+      <c r="H377" s="3">
+        <v>3003.0</v>
+      </c>
+      <c r="I377" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J377" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" s="1">
+        <v>377.0</v>
+      </c>
+      <c r="B378" s="2">
+        <v>45317.621770833335</v>
+      </c>
+      <c r="C378" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="D378" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E378" s="1">
+        <v>20.0</v>
+      </c>
+      <c r="F378" s="1">
+        <v>899.99</v>
+      </c>
+      <c r="H378" s="3">
+        <v>17999.8</v>
+      </c>
+      <c r="I378" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J378" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" s="1">
+        <v>378.0</v>
+      </c>
+      <c r="B379" s="2">
+        <v>45322.471134259256</v>
+      </c>
+      <c r="C379" s="1">
+        <v>23.0</v>
+      </c>
+      <c r="D379" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E379" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="F379" s="1">
+        <v>450.5</v>
+      </c>
+      <c r="H379" s="1">
+        <v>1351.5</v>
+      </c>
+      <c r="I379" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J379" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" s="1">
+        <v>379.0</v>
+      </c>
+      <c r="B380" s="2">
+        <v>45323.38385416667</v>
+      </c>
+      <c r="C380" s="1">
+        <v>445.0</v>
+      </c>
+      <c r="D380" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E380" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="F380" s="1">
+        <v>699.99</v>
+      </c>
+      <c r="H380" s="1">
+        <v>3499.95</v>
+      </c>
+      <c r="I380" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J380" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" s="1">
+        <v>380.0</v>
+      </c>
+      <c r="B381" s="2">
+        <v>45324.47520833334</v>
+      </c>
+      <c r="C381" s="1">
+        <v>446.0</v>
+      </c>
+      <c r="D381" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E381" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="F381" s="1">
+        <v>1350.75</v>
+      </c>
+      <c r="H381" s="1">
+        <v>2701.5</v>
+      </c>
+      <c r="I381" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J381" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" s="1">
+        <v>381.0</v>
+      </c>
+      <c r="B382" s="2">
+        <v>45325.607777777775</v>
+      </c>
+      <c r="C382" s="1">
+        <v>447.0</v>
+      </c>
+      <c r="D382" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E382" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="F382" s="1">
+        <v>1200.5</v>
+      </c>
+      <c r="H382" s="1">
+        <v>3601.5</v>
+      </c>
+      <c r="I382" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J382" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" s="1">
+        <v>382.0</v>
+      </c>
+      <c r="B383" s="2">
+        <v>45327.699641203704</v>
+      </c>
+      <c r="C383" s="1">
+        <v>448.0</v>
+      </c>
+      <c r="D383" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E383" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="F383" s="1">
+        <v>849.99</v>
+      </c>
+      <c r="H383" s="1">
+        <v>3399.96</v>
+      </c>
+      <c r="I383" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J383" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" s="1">
+        <v>383.0</v>
+      </c>
+      <c r="B384" s="2">
+        <v>45329.830509259256</v>
+      </c>
+      <c r="C384" s="1">
+        <v>449.0</v>
+      </c>
+      <c r="D384" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E384" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="F384" s="1">
+        <v>599.99</v>
+      </c>
+      <c r="H384" s="1">
+        <v>2999.95</v>
+      </c>
+      <c r="I384" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J384" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" s="1">
+        <v>384.0</v>
+      </c>
+      <c r="B385" s="2">
+        <v>45331.43315972222</v>
+      </c>
+      <c r="C385" s="1">
+        <v>450.0</v>
+      </c>
+      <c r="D385" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E385" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="F385" s="1">
+        <v>750.75</v>
+      </c>
+      <c r="H385" s="1">
+        <v>2252.25</v>
+      </c>
+      <c r="I385" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J385" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" s="1">
+        <v>385.0</v>
+      </c>
+      <c r="B386" s="2">
+        <v>45333.50795138889</v>
+      </c>
+      <c r="C386" s="1">
+        <v>451.0</v>
+      </c>
+      <c r="D386" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E386" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="F386" s="1">
+        <v>679.99</v>
+      </c>
+      <c r="H386" s="1">
+        <v>4079.94</v>
+      </c>
+      <c r="I386" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J386" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" s="1">
+        <v>386.0</v>
+      </c>
+      <c r="B387" s="2">
+        <v>45335.66646990741</v>
+      </c>
+      <c r="C387" s="1">
+        <v>452.0</v>
+      </c>
+      <c r="D387" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E387" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="F387" s="1">
+        <v>1149.99</v>
+      </c>
+      <c r="H387" s="1">
+        <v>2299.98</v>
+      </c>
+      <c r="I387" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J387" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" s="1">
+        <v>387.0</v>
+      </c>
+      <c r="B388" s="2">
+        <v>45337.73287037037</v>
+      </c>
+      <c r="C388" s="1">
+        <v>453.0</v>
+      </c>
+      <c r="D388" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E388" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="F388" s="1">
+        <v>450.5</v>
+      </c>
+      <c r="H388" s="1">
+        <v>1802.0</v>
+      </c>
+      <c r="I388" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J388" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" s="1">
+        <v>388.0</v>
+      </c>
+      <c r="B389" s="2">
+        <v>45339.40646990741</v>
+      </c>
+      <c r="C389" s="1">
+        <v>454.0</v>
+      </c>
+      <c r="D389" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E389" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="F389" s="1">
+        <v>1350.75</v>
+      </c>
+      <c r="H389" s="1">
+        <v>1350.75</v>
+      </c>
+      <c r="I389" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J389" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" s="1">
+        <v>389.0</v>
+      </c>
+      <c r="B390" s="2">
+        <v>45341.474652777775</v>
+      </c>
+      <c r="C390" s="1">
+        <v>455.0</v>
+      </c>
+      <c r="D390" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E390" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="F390" s="1">
+        <v>899.99</v>
+      </c>
+      <c r="H390" s="1">
+        <v>2699.97</v>
+      </c>
+      <c r="I390" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J390" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" s="1">
+        <v>390.0</v>
+      </c>
+      <c r="B391" s="2">
+        <v>45343.57150462963</v>
+      </c>
+      <c r="C391" s="1">
+        <v>456.0</v>
+      </c>
+      <c r="D391" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E391" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="F391" s="1">
+        <v>599.99</v>
+      </c>
+      <c r="H391" s="1">
+        <v>2399.96</v>
+      </c>
+      <c r="I391" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J391" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" s="1">
+        <v>391.0</v>
+      </c>
+      <c r="B392" s="2">
+        <v>45345.662881944445</v>
+      </c>
+      <c r="C392" s="1">
+        <v>457.0</v>
+      </c>
+      <c r="D392" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E392" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="F392" s="1">
+        <v>699.99</v>
+      </c>
+      <c r="H392" s="1">
+        <v>3499.95</v>
+      </c>
+      <c r="I392" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J392" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" s="1">
+        <v>392.0</v>
+      </c>
+      <c r="B393" s="2">
+        <v>45347.73075231481</v>
+      </c>
+      <c r="C393" s="1">
+        <v>458.0</v>
+      </c>
+      <c r="D393" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E393" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="F393" s="1">
+        <v>1199.99</v>
+      </c>
+      <c r="H393" s="1">
+        <v>3599.97</v>
+      </c>
+      <c r="I393" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J393" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" s="1">
+        <v>393.0</v>
+      </c>
+      <c r="B394" s="2">
+        <v>45349.40898148148</v>
+      </c>
+      <c r="C394" s="1">
+        <v>459.0</v>
+      </c>
+      <c r="D394" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E394" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="F394" s="1">
+        <v>750.75</v>
+      </c>
+      <c r="H394" s="1">
+        <v>1501.5</v>
+      </c>
+      <c r="I394" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J394" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" s="1">
+        <v>394.0</v>
+      </c>
+      <c r="B395" s="2">
+        <v>45351.42998842592</v>
+      </c>
+      <c r="C395" s="1">
+        <v>460.0</v>
+      </c>
+      <c r="D395" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E395" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="F395" s="1">
+        <v>849.99</v>
+      </c>
+      <c r="H395" s="1">
+        <v>3399.96</v>
+      </c>
+      <c r="I395" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J395" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="$A$1:$J$395"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>